<commit_message>
added withdraw and transfer functionality
</commit_message>
<xml_diff>
--- a/users_info.xlsx
+++ b/users_info.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6605DA7-03D7-40DD-B25B-FC7E2B1F3D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,20 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Wasif Ali</t>
   </si>
   <si>
-    <t>37102-3744962-9</t>
-  </si>
-  <si>
     <t>Student</t>
   </si>
   <si>
-    <t>66302-2334231-4</t>
-  </si>
-  <si>
     <t>Savings</t>
   </si>
   <si>
@@ -51,16 +46,10 @@
     <t>Huma Laila</t>
   </si>
   <si>
-    <t>64012-8593820-1</t>
-  </si>
-  <si>
     <t>huma.jpg</t>
   </si>
   <si>
     <t>Huzaifa Abbasi</t>
-  </si>
-  <si>
-    <t>66123-7847445-4</t>
   </si>
   <si>
     <t>huzaifa.jpg</t>
@@ -69,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,31 +369,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
+      <c r="C1">
+        <v>3710237</v>
       </c>
       <c r="D1">
         <v>40000</v>
@@ -413,24 +402,24 @@
         <v>6264</v>
       </c>
       <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
       </c>
       <c r="B2">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="C2">
+        <v>6630298</v>
       </c>
       <c r="D2">
         <v>2000000</v>
@@ -439,24 +428,24 @@
         <v>8181</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
+      <c r="C3">
+        <v>6401285</v>
       </c>
       <c r="D3">
         <v>10000000</v>
@@ -465,24 +454,24 @@
         <v>1122</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
+      <c r="C4">
+        <v>6612387</v>
       </c>
       <c r="D4">
         <v>299245</v>
@@ -491,13 +480,13 @@
         <v>8080</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Money can be transfered bw accounts now - WasifAli
</commit_message>
<xml_diff>
--- a/users_info.xlsx
+++ b/users_info.xlsx
@@ -1,76 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6605DA7-03D7-40DD-B25B-FC7E2B1F3D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
-  <si>
-    <t>Wasif Ali</t>
-  </si>
-  <si>
-    <t>Student</t>
-  </si>
-  <si>
-    <t>Savings</t>
-  </si>
-  <si>
-    <t>Current</t>
-  </si>
-  <si>
-    <t>Marium Ilyas</t>
-  </si>
-  <si>
-    <t>wasifali.jpg</t>
-  </si>
-  <si>
-    <t>marium.jpg</t>
-  </si>
-  <si>
-    <t>Huma Laila</t>
-  </si>
-  <si>
-    <t>huma.jpg</t>
-  </si>
-  <si>
-    <t>Huzaifa Abbasi</t>
-  </si>
-  <si>
-    <t>huzaifa.jpg</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -89,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -369,124 +385,160 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col width="14.140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="3" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="15.5703125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="15.28515625" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="13.42578125" bestFit="1" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Wasif Ali</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
         <v>18</v>
       </c>
-      <c r="C1">
+      <c r="C1" t="n">
         <v>3710237</v>
       </c>
-      <c r="D1">
-        <v>40000</v>
-      </c>
-      <c r="E1">
+      <c r="D1" t="n">
+        <v>50500</v>
+      </c>
+      <c r="E1" t="n">
         <v>6264</v>
       </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Savings</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>wasifali.jpg</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Marium Ilyas</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>25</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>6630298</v>
       </c>
-      <c r="D2">
-        <v>2000000</v>
-      </c>
-      <c r="E2">
+      <c r="D2" t="n">
+        <v>1989500</v>
+      </c>
+      <c r="E2" t="n">
         <v>8181</v>
       </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Current</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>marium.jpg</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Huma Laila</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>18</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>6401285</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>10000000</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>1122</v>
       </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Savings</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>huma.jpg</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Huzaifa Abbasi</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>20</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>6612387</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>299245</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>8080</v>
       </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Savings</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>huzaifa.jpg</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes - last commit today
</commit_message>
<xml_diff>
--- a/users_info.xlsx
+++ b/users_info.xlsx
@@ -418,7 +418,7 @@
         <v>3710237</v>
       </c>
       <c r="D1" t="n">
-        <v>50500</v>
+        <v>50745</v>
       </c>
       <c r="E1" t="n">
         <v>6264</v>
@@ -520,7 +520,7 @@
         <v>6612387</v>
       </c>
       <c r="D4" t="n">
-        <v>299245</v>
+        <v>299000</v>
       </c>
       <c r="E4" t="n">
         <v>8080</v>

</xml_diff>

<commit_message>
added the withdraw functionality
</commit_message>
<xml_diff>
--- a/users_info.xlsx
+++ b/users_info.xlsx
@@ -396,7 +396,7 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="14.140625" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="3" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -418,7 +418,7 @@
         <v>3710237</v>
       </c>
       <c r="D1" t="n">
-        <v>55745</v>
+        <v>54000</v>
       </c>
       <c r="E1" t="n">
         <v>6264</v>

</xml_diff>